<commit_message>
testprep: create multiple tables for quiz and modeltest in the same DB
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/modeltest_v1.xlsx
+++ b/app/src/main/res/raw/modeltest_v1.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="modeltest1" sheetId="1" r:id="rId1"/>
+    <sheet name="modeltest2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -3213,9 +3213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3301,8 +3299,12 @@
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
+      </c>
       <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -3337,8 +3339,12 @@
       <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="L3" s="10">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1</v>
+      </c>
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3373,8 +3379,12 @@
       <c r="K4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1</v>
+      </c>
       <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3409,8 +3419,12 @@
       <c r="K5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1</v>
+      </c>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3445,8 +3459,12 @@
       <c r="K6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="L6" s="10">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3481,8 +3499,12 @@
       <c r="K7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3517,8 +3539,12 @@
       <c r="K8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10">
+        <v>1</v>
+      </c>
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3553,8 +3579,12 @@
       <c r="K9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="L9" s="10">
+        <v>1</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1</v>
+      </c>
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3589,8 +3619,12 @@
       <c r="K10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="L10" s="10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10">
+        <v>1</v>
+      </c>
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3625,8 +3659,12 @@
       <c r="K11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
+      <c r="L11" s="10">
+        <v>1</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1</v>
+      </c>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3661,8 +3699,12 @@
       <c r="K12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="L12" s="10">
+        <v>1</v>
+      </c>
+      <c r="M12" s="10">
+        <v>1</v>
+      </c>
       <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3697,8 +3739,12 @@
       <c r="K13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
+      <c r="M13" s="10">
+        <v>1</v>
+      </c>
       <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3733,8 +3779,12 @@
       <c r="K14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
+      <c r="M14" s="10">
+        <v>1</v>
+      </c>
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3769,8 +3819,12 @@
       <c r="K15" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="L15" s="10">
+        <v>1</v>
+      </c>
+      <c r="M15" s="10">
+        <v>1</v>
+      </c>
       <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3805,8 +3859,12 @@
       <c r="K16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="10">
+        <v>1</v>
+      </c>
       <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -3841,8 +3899,12 @@
       <c r="K17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
+      <c r="M17" s="10">
+        <v>1</v>
+      </c>
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3877,8 +3939,12 @@
       <c r="K18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="L18" s="10">
+        <v>1</v>
+      </c>
+      <c r="M18" s="10">
+        <v>1</v>
+      </c>
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -3913,8 +3979,12 @@
       <c r="K19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="L19" s="10">
+        <v>1</v>
+      </c>
+      <c r="M19" s="10">
+        <v>1</v>
+      </c>
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -3949,8 +4019,12 @@
       <c r="K20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
+        <v>1</v>
+      </c>
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3985,8 +4059,12 @@
       <c r="K21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="L21" s="10">
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
+        <v>1</v>
+      </c>
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4021,8 +4099,12 @@
       <c r="K22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
+      <c r="L22" s="10">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10">
+        <v>1</v>
+      </c>
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -4057,8 +4139,12 @@
       <c r="K23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="L23" s="10">
+        <v>1</v>
+      </c>
+      <c r="M23" s="10">
+        <v>1</v>
+      </c>
       <c r="N23" s="10"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -4093,8 +4179,12 @@
       <c r="K24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="L24" s="10">
+        <v>1</v>
+      </c>
+      <c r="M24" s="10">
+        <v>1</v>
+      </c>
       <c r="N24" s="10"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -4129,8 +4219,12 @@
       <c r="K25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
+      <c r="M25" s="10">
+        <v>1</v>
+      </c>
       <c r="N25" s="10"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -4165,8 +4259,12 @@
       <c r="K26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10">
+        <v>1</v>
+      </c>
       <c r="N26" s="10"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -4201,8 +4299,12 @@
       <c r="K27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
+      <c r="L27" s="10">
+        <v>1</v>
+      </c>
+      <c r="M27" s="10">
+        <v>1</v>
+      </c>
       <c r="N27" s="10"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -4237,8 +4339,12 @@
       <c r="K28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="L28" s="10">
+        <v>1</v>
+      </c>
+      <c r="M28" s="10">
+        <v>1</v>
+      </c>
       <c r="N28" s="10"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -4273,8 +4379,12 @@
       <c r="K29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="10">
+        <v>1</v>
+      </c>
+      <c r="M29" s="10">
+        <v>1</v>
+      </c>
       <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -4309,8 +4419,12 @@
       <c r="K30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
+      <c r="L30" s="10">
+        <v>1</v>
+      </c>
+      <c r="M30" s="10">
+        <v>1</v>
+      </c>
       <c r="N30" s="10"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -4345,8 +4459,12 @@
       <c r="K31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="L31" s="10">
+        <v>1</v>
+      </c>
+      <c r="M31" s="10">
+        <v>1</v>
+      </c>
       <c r="N31" s="10"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -4381,8 +4499,12 @@
       <c r="K32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="L32" s="10">
+        <v>1</v>
+      </c>
+      <c r="M32" s="10">
+        <v>1</v>
+      </c>
       <c r="N32" s="10"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -4417,8 +4539,12 @@
       <c r="K33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
+      <c r="L33" s="10">
+        <v>1</v>
+      </c>
+      <c r="M33" s="10">
+        <v>1</v>
+      </c>
       <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4453,8 +4579,12 @@
       <c r="K34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
+      <c r="L34" s="10">
+        <v>1</v>
+      </c>
+      <c r="M34" s="10">
+        <v>1</v>
+      </c>
       <c r="N34" s="10"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4489,8 +4619,12 @@
       <c r="K35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
+      <c r="L35" s="10">
+        <v>1</v>
+      </c>
+      <c r="M35" s="10">
+        <v>1</v>
+      </c>
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -4525,8 +4659,12 @@
       <c r="K36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
+      <c r="L36" s="10">
+        <v>1</v>
+      </c>
+      <c r="M36" s="10">
+        <v>1</v>
+      </c>
       <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4561,8 +4699,12 @@
       <c r="K37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
+      <c r="L37" s="10">
+        <v>1</v>
+      </c>
+      <c r="M37" s="10">
+        <v>1</v>
+      </c>
       <c r="N37" s="10"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -4597,8 +4739,12 @@
       <c r="K38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
+      <c r="L38" s="10">
+        <v>1</v>
+      </c>
+      <c r="M38" s="10">
+        <v>1</v>
+      </c>
       <c r="N38" s="10"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4633,8 +4779,12 @@
       <c r="K39" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
+      <c r="L39" s="10">
+        <v>1</v>
+      </c>
+      <c r="M39" s="10">
+        <v>1</v>
+      </c>
       <c r="N39" s="10"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -4669,8 +4819,12 @@
       <c r="K40" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
+      <c r="L40" s="10">
+        <v>1</v>
+      </c>
+      <c r="M40" s="10">
+        <v>1</v>
+      </c>
       <c r="N40" s="10"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -4705,8 +4859,12 @@
       <c r="K41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
+      <c r="L41" s="10">
+        <v>1</v>
+      </c>
+      <c r="M41" s="10">
+        <v>1</v>
+      </c>
       <c r="N41" s="10"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4741,8 +4899,12 @@
       <c r="K42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
+      <c r="L42" s="10">
+        <v>1</v>
+      </c>
+      <c r="M42" s="10">
+        <v>1</v>
+      </c>
       <c r="N42" s="10"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -4777,8 +4939,12 @@
       <c r="K43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
+      <c r="L43" s="10">
+        <v>1</v>
+      </c>
+      <c r="M43" s="10">
+        <v>1</v>
+      </c>
       <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -4813,8 +4979,12 @@
       <c r="K44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
+      <c r="L44" s="10">
+        <v>1</v>
+      </c>
+      <c r="M44" s="10">
+        <v>1</v>
+      </c>
       <c r="N44" s="10"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -4849,8 +5019,12 @@
       <c r="K45" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
+      <c r="L45" s="10">
+        <v>1</v>
+      </c>
+      <c r="M45" s="10">
+        <v>1</v>
+      </c>
       <c r="N45" s="10"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -4885,8 +5059,12 @@
       <c r="K46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
+      <c r="L46" s="10">
+        <v>1</v>
+      </c>
+      <c r="M46" s="10">
+        <v>1</v>
+      </c>
       <c r="N46" s="10"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -4921,8 +5099,12 @@
       <c r="K47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
+      <c r="L47" s="10">
+        <v>1</v>
+      </c>
+      <c r="M47" s="10">
+        <v>1</v>
+      </c>
       <c r="N47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4957,8 +5139,12 @@
       <c r="K48" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
+      <c r="L48" s="10">
+        <v>1</v>
+      </c>
+      <c r="M48" s="10">
+        <v>1</v>
+      </c>
       <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -4993,8 +5179,12 @@
       <c r="K49" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
+      <c r="L49" s="10">
+        <v>1</v>
+      </c>
+      <c r="M49" s="10">
+        <v>1</v>
+      </c>
       <c r="N49" s="10"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -5029,8 +5219,12 @@
       <c r="K50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
+      <c r="L50" s="10">
+        <v>1</v>
+      </c>
+      <c r="M50" s="10">
+        <v>1</v>
+      </c>
       <c r="N50" s="10"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -5065,8 +5259,12 @@
       <c r="K51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
+      <c r="L51" s="10">
+        <v>1</v>
+      </c>
+      <c r="M51" s="10">
+        <v>1</v>
+      </c>
       <c r="N51" s="10"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -5101,8 +5299,12 @@
       <c r="K52" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
+      <c r="L52" s="10">
+        <v>1</v>
+      </c>
+      <c r="M52" s="10">
+        <v>1</v>
+      </c>
       <c r="N52" s="10"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -5137,8 +5339,12 @@
       <c r="K53" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
+      <c r="L53" s="10">
+        <v>1</v>
+      </c>
+      <c r="M53" s="10">
+        <v>1</v>
+      </c>
       <c r="N53" s="10"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -5173,8 +5379,12 @@
       <c r="K54" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L54" s="10"/>
-      <c r="M54" s="10"/>
+      <c r="L54" s="10">
+        <v>1</v>
+      </c>
+      <c r="M54" s="10">
+        <v>1</v>
+      </c>
       <c r="N54" s="10"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -5209,8 +5419,12 @@
       <c r="K55" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
+      <c r="L55" s="10">
+        <v>1</v>
+      </c>
+      <c r="M55" s="10">
+        <v>1</v>
+      </c>
       <c r="N55" s="10"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -5245,8 +5459,12 @@
       <c r="K56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
+      <c r="L56" s="10">
+        <v>1</v>
+      </c>
+      <c r="M56" s="10">
+        <v>1</v>
+      </c>
       <c r="N56" s="10"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -5281,8 +5499,12 @@
       <c r="K57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L57" s="10"/>
-      <c r="M57" s="10"/>
+      <c r="L57" s="10">
+        <v>1</v>
+      </c>
+      <c r="M57" s="10">
+        <v>1</v>
+      </c>
       <c r="N57" s="10"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -5317,8 +5539,12 @@
       <c r="K58" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
+      <c r="L58" s="10">
+        <v>1</v>
+      </c>
+      <c r="M58" s="10">
+        <v>1</v>
+      </c>
       <c r="N58" s="10"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -5353,8 +5579,12 @@
       <c r="K59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
+      <c r="L59" s="10">
+        <v>1</v>
+      </c>
+      <c r="M59" s="10">
+        <v>1</v>
+      </c>
       <c r="N59" s="10"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -5389,8 +5619,12 @@
       <c r="K60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L60" s="10"/>
-      <c r="M60" s="10"/>
+      <c r="L60" s="10">
+        <v>1</v>
+      </c>
+      <c r="M60" s="10">
+        <v>1</v>
+      </c>
       <c r="N60" s="10"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -5425,8 +5659,12 @@
       <c r="K61" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
+      <c r="L61" s="10">
+        <v>1</v>
+      </c>
+      <c r="M61" s="10">
+        <v>1</v>
+      </c>
       <c r="N61" s="10"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -5461,8 +5699,12 @@
       <c r="K62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
+      <c r="L62" s="10">
+        <v>1</v>
+      </c>
+      <c r="M62" s="10">
+        <v>1</v>
+      </c>
       <c r="N62" s="10"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -5497,8 +5739,12 @@
       <c r="K63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
+      <c r="L63" s="10">
+        <v>1</v>
+      </c>
+      <c r="M63" s="10">
+        <v>1</v>
+      </c>
       <c r="N63" s="10"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -5533,8 +5779,12 @@
       <c r="K64" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
+      <c r="L64" s="10">
+        <v>1</v>
+      </c>
+      <c r="M64" s="10">
+        <v>1</v>
+      </c>
       <c r="N64" s="10"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -5569,8 +5819,12 @@
       <c r="K65" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L65" s="10"/>
-      <c r="M65" s="10"/>
+      <c r="L65" s="10">
+        <v>1</v>
+      </c>
+      <c r="M65" s="10">
+        <v>1</v>
+      </c>
       <c r="N65" s="10"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -5605,8 +5859,12 @@
       <c r="K66" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L66" s="10"/>
-      <c r="M66" s="10"/>
+      <c r="L66" s="10">
+        <v>1</v>
+      </c>
+      <c r="M66" s="10">
+        <v>1</v>
+      </c>
       <c r="N66" s="10"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -5641,8 +5899,12 @@
       <c r="K67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L67" s="10"/>
-      <c r="M67" s="10"/>
+      <c r="L67" s="10">
+        <v>1</v>
+      </c>
+      <c r="M67" s="10">
+        <v>1</v>
+      </c>
       <c r="N67" s="10"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -5677,8 +5939,12 @@
       <c r="K68" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L68" s="10"/>
-      <c r="M68" s="10"/>
+      <c r="L68" s="10">
+        <v>1</v>
+      </c>
+      <c r="M68" s="10">
+        <v>1</v>
+      </c>
       <c r="N68" s="10"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -5713,8 +5979,12 @@
       <c r="K69" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L69" s="10"/>
-      <c r="M69" s="10"/>
+      <c r="L69" s="10">
+        <v>1</v>
+      </c>
+      <c r="M69" s="10">
+        <v>1</v>
+      </c>
       <c r="N69" s="10"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -5749,8 +6019,12 @@
       <c r="K70" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L70" s="10"/>
-      <c r="M70" s="10"/>
+      <c r="L70" s="10">
+        <v>1</v>
+      </c>
+      <c r="M70" s="10">
+        <v>1</v>
+      </c>
       <c r="N70" s="10"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -5785,8 +6059,12 @@
       <c r="K71" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
+      <c r="L71" s="10">
+        <v>1</v>
+      </c>
+      <c r="M71" s="10">
+        <v>1</v>
+      </c>
       <c r="N71" s="10"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -5821,8 +6099,12 @@
       <c r="K72" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L72" s="10"/>
-      <c r="M72" s="10"/>
+      <c r="L72" s="10">
+        <v>1</v>
+      </c>
+      <c r="M72" s="10">
+        <v>1</v>
+      </c>
       <c r="N72" s="10"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -5857,8 +6139,12 @@
       <c r="K73" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L73" s="10"/>
-      <c r="M73" s="10"/>
+      <c r="L73" s="10">
+        <v>1</v>
+      </c>
+      <c r="M73" s="10">
+        <v>1</v>
+      </c>
       <c r="N73" s="10"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -5893,8 +6179,12 @@
       <c r="K74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L74" s="10"/>
-      <c r="M74" s="10"/>
+      <c r="L74" s="10">
+        <v>1</v>
+      </c>
+      <c r="M74" s="10">
+        <v>1</v>
+      </c>
       <c r="N74" s="10"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -5929,8 +6219,12 @@
       <c r="K75" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L75" s="10"/>
-      <c r="M75" s="10"/>
+      <c r="L75" s="10">
+        <v>1</v>
+      </c>
+      <c r="M75" s="10">
+        <v>1</v>
+      </c>
       <c r="N75" s="10"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -5965,8 +6259,12 @@
       <c r="K76" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L76" s="10"/>
-      <c r="M76" s="10"/>
+      <c r="L76" s="10">
+        <v>1</v>
+      </c>
+      <c r="M76" s="10">
+        <v>1</v>
+      </c>
       <c r="N76" s="10"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -6001,8 +6299,12 @@
       <c r="K77" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L77" s="10"/>
-      <c r="M77" s="10"/>
+      <c r="L77" s="10">
+        <v>1</v>
+      </c>
+      <c r="M77" s="10">
+        <v>1</v>
+      </c>
       <c r="N77" s="10"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -6037,8 +6339,12 @@
       <c r="K78" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
+      <c r="L78" s="10">
+        <v>1</v>
+      </c>
+      <c r="M78" s="10">
+        <v>1</v>
+      </c>
       <c r="N78" s="10"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -6073,8 +6379,12 @@
       <c r="K79" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
+      <c r="L79" s="10">
+        <v>1</v>
+      </c>
+      <c r="M79" s="10">
+        <v>1</v>
+      </c>
       <c r="N79" s="10"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -6109,8 +6419,12 @@
       <c r="K80" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L80" s="10"/>
-      <c r="M80" s="10"/>
+      <c r="L80" s="10">
+        <v>1</v>
+      </c>
+      <c r="M80" s="10">
+        <v>1</v>
+      </c>
       <c r="N80" s="10"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -6145,8 +6459,12 @@
       <c r="K81" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L81" s="10"/>
-      <c r="M81" s="10"/>
+      <c r="L81" s="10">
+        <v>1</v>
+      </c>
+      <c r="M81" s="10">
+        <v>1</v>
+      </c>
       <c r="N81" s="10"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -6181,8 +6499,12 @@
       <c r="K82" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L82" s="10"/>
-      <c r="M82" s="10"/>
+      <c r="L82" s="10">
+        <v>1</v>
+      </c>
+      <c r="M82" s="10">
+        <v>1</v>
+      </c>
       <c r="N82" s="10"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -6217,8 +6539,12 @@
       <c r="K83" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
+      <c r="L83" s="10">
+        <v>1</v>
+      </c>
+      <c r="M83" s="10">
+        <v>1</v>
+      </c>
       <c r="N83" s="10"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -6253,8 +6579,12 @@
       <c r="K84" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L84" s="10"/>
-      <c r="M84" s="10"/>
+      <c r="L84" s="10">
+        <v>1</v>
+      </c>
+      <c r="M84" s="10">
+        <v>1</v>
+      </c>
       <c r="N84" s="10"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -6289,8 +6619,12 @@
       <c r="K85" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
+      <c r="L85" s="10">
+        <v>1</v>
+      </c>
+      <c r="M85" s="10">
+        <v>1</v>
+      </c>
       <c r="N85" s="10"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -6325,8 +6659,12 @@
       <c r="K86" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L86" s="10"/>
-      <c r="M86" s="10"/>
+      <c r="L86" s="10">
+        <v>1</v>
+      </c>
+      <c r="M86" s="10">
+        <v>1</v>
+      </c>
       <c r="N86" s="10"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -6361,8 +6699,12 @@
       <c r="K87" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L87" s="10"/>
-      <c r="M87" s="10"/>
+      <c r="L87" s="10">
+        <v>1</v>
+      </c>
+      <c r="M87" s="10">
+        <v>1</v>
+      </c>
       <c r="N87" s="10"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -6397,8 +6739,12 @@
       <c r="K88" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
+      <c r="L88" s="10">
+        <v>1</v>
+      </c>
+      <c r="M88" s="10">
+        <v>1</v>
+      </c>
       <c r="N88" s="10"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -6433,8 +6779,12 @@
       <c r="K89" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
+      <c r="L89" s="10">
+        <v>1</v>
+      </c>
+      <c r="M89" s="10">
+        <v>1</v>
+      </c>
       <c r="N89" s="10"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -6469,8 +6819,12 @@
       <c r="K90" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
+      <c r="L90" s="10">
+        <v>1</v>
+      </c>
+      <c r="M90" s="10">
+        <v>1</v>
+      </c>
       <c r="N90" s="10"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -6505,8 +6859,12 @@
       <c r="K91" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L91" s="10"/>
-      <c r="M91" s="10"/>
+      <c r="L91" s="10">
+        <v>1</v>
+      </c>
+      <c r="M91" s="10">
+        <v>1</v>
+      </c>
       <c r="N91" s="10"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -6541,8 +6899,12 @@
       <c r="K92" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L92" s="10"/>
-      <c r="M92" s="10"/>
+      <c r="L92" s="10">
+        <v>1</v>
+      </c>
+      <c r="M92" s="10">
+        <v>1</v>
+      </c>
       <c r="N92" s="10"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -6577,8 +6939,12 @@
       <c r="K93" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L93" s="10"/>
-      <c r="M93" s="10"/>
+      <c r="L93" s="10">
+        <v>1</v>
+      </c>
+      <c r="M93" s="10">
+        <v>1</v>
+      </c>
       <c r="N93" s="10"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -6613,8 +6979,12 @@
       <c r="K94" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L94" s="10"/>
-      <c r="M94" s="10"/>
+      <c r="L94" s="10">
+        <v>1</v>
+      </c>
+      <c r="M94" s="10">
+        <v>1</v>
+      </c>
       <c r="N94" s="10"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -6649,8 +7019,12 @@
       <c r="K95" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L95" s="10"/>
-      <c r="M95" s="10"/>
+      <c r="L95" s="10">
+        <v>1</v>
+      </c>
+      <c r="M95" s="10">
+        <v>1</v>
+      </c>
       <c r="N95" s="10"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -6685,8 +7059,12 @@
       <c r="K96" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L96" s="10"/>
-      <c r="M96" s="10"/>
+      <c r="L96" s="10">
+        <v>1</v>
+      </c>
+      <c r="M96" s="10">
+        <v>1</v>
+      </c>
       <c r="N96" s="10"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -6721,8 +7099,12 @@
       <c r="K97" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L97" s="10"/>
-      <c r="M97" s="10"/>
+      <c r="L97" s="10">
+        <v>1</v>
+      </c>
+      <c r="M97" s="10">
+        <v>1</v>
+      </c>
       <c r="N97" s="10"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -6757,8 +7139,12 @@
       <c r="K98" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L98" s="10"/>
-      <c r="M98" s="10"/>
+      <c r="L98" s="10">
+        <v>1</v>
+      </c>
+      <c r="M98" s="10">
+        <v>1</v>
+      </c>
       <c r="N98" s="10"/>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -6793,8 +7179,12 @@
       <c r="K99" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L99" s="10"/>
-      <c r="M99" s="10"/>
+      <c r="L99" s="10">
+        <v>1</v>
+      </c>
+      <c r="M99" s="10">
+        <v>1</v>
+      </c>
       <c r="N99" s="10"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -6829,8 +7219,12 @@
       <c r="K100" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L100" s="10"/>
-      <c r="M100" s="10"/>
+      <c r="L100" s="10">
+        <v>1</v>
+      </c>
+      <c r="M100" s="10">
+        <v>1</v>
+      </c>
       <c r="N100" s="10"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -6865,8 +7259,12 @@
       <c r="K101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L101" s="10"/>
-      <c r="M101" s="10"/>
+      <c r="L101" s="10">
+        <v>1</v>
+      </c>
+      <c r="M101" s="10">
+        <v>1</v>
+      </c>
       <c r="N101" s="10"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -6901,8 +7299,12 @@
       <c r="K102" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L102" s="10"/>
-      <c r="M102" s="10"/>
+      <c r="L102" s="10">
+        <v>1</v>
+      </c>
+      <c r="M102" s="10">
+        <v>1</v>
+      </c>
       <c r="N102" s="10"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -6937,8 +7339,12 @@
       <c r="K103" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L103" s="10"/>
-      <c r="M103" s="10"/>
+      <c r="L103" s="10">
+        <v>1</v>
+      </c>
+      <c r="M103" s="10">
+        <v>1</v>
+      </c>
       <c r="N103" s="10"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -6973,8 +7379,12 @@
       <c r="K104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L104" s="10"/>
-      <c r="M104" s="10"/>
+      <c r="L104" s="10">
+        <v>1</v>
+      </c>
+      <c r="M104" s="10">
+        <v>1</v>
+      </c>
       <c r="N104" s="10"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -7009,8 +7419,12 @@
       <c r="K105" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L105" s="10"/>
-      <c r="M105" s="10"/>
+      <c r="L105" s="10">
+        <v>1</v>
+      </c>
+      <c r="M105" s="10">
+        <v>1</v>
+      </c>
       <c r="N105" s="10"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -7045,8 +7459,12 @@
       <c r="K106" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L106" s="10"/>
-      <c r="M106" s="10"/>
+      <c r="L106" s="10">
+        <v>1</v>
+      </c>
+      <c r="M106" s="10">
+        <v>1</v>
+      </c>
       <c r="N106" s="10"/>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -7081,8 +7499,12 @@
       <c r="K107" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L107" s="10"/>
-      <c r="M107" s="10"/>
+      <c r="L107" s="10">
+        <v>1</v>
+      </c>
+      <c r="M107" s="10">
+        <v>1</v>
+      </c>
       <c r="N107" s="10"/>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -7117,8 +7539,12 @@
       <c r="K108" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L108" s="10"/>
-      <c r="M108" s="10"/>
+      <c r="L108" s="10">
+        <v>1</v>
+      </c>
+      <c r="M108" s="10">
+        <v>1</v>
+      </c>
       <c r="N108" s="10"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -7153,8 +7579,12 @@
       <c r="K109" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L109" s="10"/>
-      <c r="M109" s="10"/>
+      <c r="L109" s="10">
+        <v>1</v>
+      </c>
+      <c r="M109" s="10">
+        <v>1</v>
+      </c>
       <c r="N109" s="10"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -7189,8 +7619,12 @@
       <c r="K110" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L110" s="10"/>
-      <c r="M110" s="10"/>
+      <c r="L110" s="10">
+        <v>1</v>
+      </c>
+      <c r="M110" s="10">
+        <v>1</v>
+      </c>
       <c r="N110" s="10"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -7225,8 +7659,12 @@
       <c r="K111" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L111" s="10"/>
-      <c r="M111" s="10"/>
+      <c r="L111" s="10">
+        <v>1</v>
+      </c>
+      <c r="M111" s="10">
+        <v>1</v>
+      </c>
       <c r="N111" s="10"/>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -7261,8 +7699,12 @@
       <c r="K112" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L112" s="10"/>
-      <c r="M112" s="10"/>
+      <c r="L112" s="10">
+        <v>1</v>
+      </c>
+      <c r="M112" s="10">
+        <v>1</v>
+      </c>
       <c r="N112" s="10"/>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -7297,8 +7739,12 @@
       <c r="K113" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L113" s="10"/>
-      <c r="M113" s="10"/>
+      <c r="L113" s="10">
+        <v>1</v>
+      </c>
+      <c r="M113" s="10">
+        <v>1</v>
+      </c>
       <c r="N113" s="10"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -7333,8 +7779,12 @@
       <c r="K114" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L114" s="10"/>
-      <c r="M114" s="10"/>
+      <c r="L114" s="10">
+        <v>1</v>
+      </c>
+      <c r="M114" s="10">
+        <v>1</v>
+      </c>
       <c r="N114" s="10"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -7369,8 +7819,12 @@
       <c r="K115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L115" s="10"/>
-      <c r="M115" s="10"/>
+      <c r="L115" s="10">
+        <v>1</v>
+      </c>
+      <c r="M115" s="10">
+        <v>1</v>
+      </c>
       <c r="N115" s="10"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -7405,8 +7859,12 @@
       <c r="K116" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L116" s="10"/>
-      <c r="M116" s="10"/>
+      <c r="L116" s="10">
+        <v>1</v>
+      </c>
+      <c r="M116" s="10">
+        <v>1</v>
+      </c>
       <c r="N116" s="10"/>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -7441,8 +7899,12 @@
       <c r="K117" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L117" s="10"/>
-      <c r="M117" s="10"/>
+      <c r="L117" s="10">
+        <v>1</v>
+      </c>
+      <c r="M117" s="10">
+        <v>1</v>
+      </c>
       <c r="N117" s="10"/>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -7477,8 +7939,12 @@
       <c r="K118" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L118" s="10"/>
-      <c r="M118" s="10"/>
+      <c r="L118" s="10">
+        <v>1</v>
+      </c>
+      <c r="M118" s="10">
+        <v>1</v>
+      </c>
       <c r="N118" s="10"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -7513,8 +7979,12 @@
       <c r="K119" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L119" s="10"/>
-      <c r="M119" s="10"/>
+      <c r="L119" s="10">
+        <v>1</v>
+      </c>
+      <c r="M119" s="10">
+        <v>1</v>
+      </c>
       <c r="N119" s="10"/>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -7549,8 +8019,12 @@
       <c r="K120" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L120" s="10"/>
-      <c r="M120" s="10"/>
+      <c r="L120" s="10">
+        <v>1</v>
+      </c>
+      <c r="M120" s="10">
+        <v>1</v>
+      </c>
       <c r="N120" s="10"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -7585,8 +8059,12 @@
       <c r="K121" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L121" s="10"/>
-      <c r="M121" s="10"/>
+      <c r="L121" s="10">
+        <v>1</v>
+      </c>
+      <c r="M121" s="10">
+        <v>1</v>
+      </c>
       <c r="N121" s="10"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -7621,8 +8099,12 @@
       <c r="K122" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L122" s="10"/>
-      <c r="M122" s="10"/>
+      <c r="L122" s="10">
+        <v>1</v>
+      </c>
+      <c r="M122" s="10">
+        <v>1</v>
+      </c>
       <c r="N122" s="10"/>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -7657,8 +8139,12 @@
       <c r="K123" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L123" s="10"/>
-      <c r="M123" s="10"/>
+      <c r="L123" s="10">
+        <v>1</v>
+      </c>
+      <c r="M123" s="10">
+        <v>1</v>
+      </c>
       <c r="N123" s="10"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
@@ -7693,8 +8179,12 @@
       <c r="K124" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L124" s="10"/>
-      <c r="M124" s="10"/>
+      <c r="L124" s="10">
+        <v>1</v>
+      </c>
+      <c r="M124" s="10">
+        <v>1</v>
+      </c>
       <c r="N124" s="10"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -7729,8 +8219,12 @@
       <c r="K125" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L125" s="10"/>
-      <c r="M125" s="10"/>
+      <c r="L125" s="10">
+        <v>1</v>
+      </c>
+      <c r="M125" s="10">
+        <v>1</v>
+      </c>
       <c r="N125" s="10"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -7765,8 +8259,12 @@
       <c r="K126" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L126" s="10"/>
-      <c r="M126" s="10"/>
+      <c r="L126" s="10">
+        <v>1</v>
+      </c>
+      <c r="M126" s="10">
+        <v>1</v>
+      </c>
       <c r="N126" s="10"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -7801,8 +8299,12 @@
       <c r="K127" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L127" s="10"/>
-      <c r="M127" s="10"/>
+      <c r="L127" s="10">
+        <v>1</v>
+      </c>
+      <c r="M127" s="10">
+        <v>1</v>
+      </c>
       <c r="N127" s="10"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -7837,8 +8339,12 @@
       <c r="K128" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L128" s="10"/>
-      <c r="M128" s="10"/>
+      <c r="L128" s="10">
+        <v>1</v>
+      </c>
+      <c r="M128" s="10">
+        <v>1</v>
+      </c>
       <c r="N128" s="10"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -7873,8 +8379,12 @@
       <c r="K129" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L129" s="10"/>
-      <c r="M129" s="10"/>
+      <c r="L129" s="10">
+        <v>1</v>
+      </c>
+      <c r="M129" s="10">
+        <v>1</v>
+      </c>
       <c r="N129" s="10"/>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -7909,8 +8419,12 @@
       <c r="K130" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L130" s="10"/>
-      <c r="M130" s="10"/>
+      <c r="L130" s="10">
+        <v>1</v>
+      </c>
+      <c r="M130" s="10">
+        <v>1</v>
+      </c>
       <c r="N130" s="10"/>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -7945,8 +8459,12 @@
       <c r="K131" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L131" s="10"/>
-      <c r="M131" s="10"/>
+      <c r="L131" s="10">
+        <v>1</v>
+      </c>
+      <c r="M131" s="10">
+        <v>1</v>
+      </c>
       <c r="N131" s="10"/>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -7981,8 +8499,12 @@
       <c r="K132" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L132" s="10"/>
-      <c r="M132" s="10"/>
+      <c r="L132" s="10">
+        <v>1</v>
+      </c>
+      <c r="M132" s="10">
+        <v>1</v>
+      </c>
       <c r="N132" s="10"/>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
@@ -8017,8 +8539,12 @@
       <c r="K133" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L133" s="10"/>
-      <c r="M133" s="10"/>
+      <c r="L133" s="10">
+        <v>1</v>
+      </c>
+      <c r="M133" s="10">
+        <v>1</v>
+      </c>
       <c r="N133" s="10"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -8053,8 +8579,12 @@
       <c r="K134" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L134" s="10"/>
-      <c r="M134" s="10"/>
+      <c r="L134" s="10">
+        <v>1</v>
+      </c>
+      <c r="M134" s="10">
+        <v>1</v>
+      </c>
       <c r="N134" s="10"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -8089,8 +8619,12 @@
       <c r="K135" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L135" s="10"/>
-      <c r="M135" s="10"/>
+      <c r="L135" s="10">
+        <v>1</v>
+      </c>
+      <c r="M135" s="10">
+        <v>1</v>
+      </c>
       <c r="N135" s="10"/>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -8125,8 +8659,12 @@
       <c r="K136" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L136" s="10"/>
-      <c r="M136" s="10"/>
+      <c r="L136" s="10">
+        <v>1</v>
+      </c>
+      <c r="M136" s="10">
+        <v>1</v>
+      </c>
       <c r="N136" s="10"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -8161,8 +8699,12 @@
       <c r="K137" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L137" s="10"/>
-      <c r="M137" s="10"/>
+      <c r="L137" s="10">
+        <v>1</v>
+      </c>
+      <c r="M137" s="10">
+        <v>1</v>
+      </c>
       <c r="N137" s="10"/>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -8197,8 +8739,12 @@
       <c r="K138" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L138" s="10"/>
-      <c r="M138" s="10"/>
+      <c r="L138" s="10">
+        <v>1</v>
+      </c>
+      <c r="M138" s="10">
+        <v>1</v>
+      </c>
       <c r="N138" s="10"/>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -8233,8 +8779,12 @@
       <c r="K139" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L139" s="10"/>
-      <c r="M139" s="10"/>
+      <c r="L139" s="10">
+        <v>1</v>
+      </c>
+      <c r="M139" s="10">
+        <v>1</v>
+      </c>
       <c r="N139" s="10"/>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -8269,8 +8819,12 @@
       <c r="K140" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L140" s="10"/>
-      <c r="M140" s="10"/>
+      <c r="L140" s="10">
+        <v>1</v>
+      </c>
+      <c r="M140" s="10">
+        <v>1</v>
+      </c>
       <c r="N140" s="10"/>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -8305,8 +8859,12 @@
       <c r="K141" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L141" s="10"/>
-      <c r="M141" s="10"/>
+      <c r="L141" s="10">
+        <v>1</v>
+      </c>
+      <c r="M141" s="10">
+        <v>1</v>
+      </c>
       <c r="N141" s="10"/>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
@@ -8341,8 +8899,12 @@
       <c r="K142" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L142" s="10"/>
-      <c r="M142" s="10"/>
+      <c r="L142" s="10">
+        <v>1</v>
+      </c>
+      <c r="M142" s="10">
+        <v>1</v>
+      </c>
       <c r="N142" s="10"/>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -8377,8 +8939,12 @@
       <c r="K143" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L143" s="10"/>
-      <c r="M143" s="10"/>
+      <c r="L143" s="10">
+        <v>1</v>
+      </c>
+      <c r="M143" s="10">
+        <v>1</v>
+      </c>
       <c r="N143" s="10"/>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -8413,8 +8979,12 @@
       <c r="K144" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L144" s="10"/>
-      <c r="M144" s="10"/>
+      <c r="L144" s="10">
+        <v>1</v>
+      </c>
+      <c r="M144" s="10">
+        <v>1</v>
+      </c>
       <c r="N144" s="10"/>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -8449,8 +9019,12 @@
       <c r="K145" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L145" s="10"/>
-      <c r="M145" s="10"/>
+      <c r="L145" s="10">
+        <v>1</v>
+      </c>
+      <c r="M145" s="10">
+        <v>1</v>
+      </c>
       <c r="N145" s="10"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -8485,8 +9059,12 @@
       <c r="K146" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L146" s="10"/>
-      <c r="M146" s="10"/>
+      <c r="L146" s="10">
+        <v>1</v>
+      </c>
+      <c r="M146" s="10">
+        <v>1</v>
+      </c>
       <c r="N146" s="10"/>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -8521,8 +9099,12 @@
       <c r="K147" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L147" s="10"/>
-      <c r="M147" s="10"/>
+      <c r="L147" s="10">
+        <v>1</v>
+      </c>
+      <c r="M147" s="10">
+        <v>1</v>
+      </c>
       <c r="N147" s="10"/>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -8557,8 +9139,12 @@
       <c r="K148" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L148" s="10"/>
-      <c r="M148" s="10"/>
+      <c r="L148" s="10">
+        <v>1</v>
+      </c>
+      <c r="M148" s="10">
+        <v>1</v>
+      </c>
       <c r="N148" s="10"/>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -8593,8 +9179,12 @@
       <c r="K149" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L149" s="10"/>
-      <c r="M149" s="10"/>
+      <c r="L149" s="10">
+        <v>1</v>
+      </c>
+      <c r="M149" s="10">
+        <v>1</v>
+      </c>
       <c r="N149" s="10"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -8629,8 +9219,12 @@
       <c r="K150" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L150" s="10"/>
-      <c r="M150" s="10"/>
+      <c r="L150" s="10">
+        <v>1</v>
+      </c>
+      <c r="M150" s="10">
+        <v>1</v>
+      </c>
       <c r="N150" s="10"/>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -8665,8 +9259,12 @@
       <c r="K151" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L151" s="10"/>
-      <c r="M151" s="10"/>
+      <c r="L151" s="10">
+        <v>1</v>
+      </c>
+      <c r="M151" s="10">
+        <v>1</v>
+      </c>
       <c r="N151" s="10"/>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
@@ -8701,8 +9299,12 @@
       <c r="K152" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L152" s="10"/>
-      <c r="M152" s="10"/>
+      <c r="L152" s="10">
+        <v>1</v>
+      </c>
+      <c r="M152" s="10">
+        <v>1</v>
+      </c>
       <c r="N152" s="10"/>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
@@ -8737,8 +9339,12 @@
       <c r="K153" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L153" s="10"/>
-      <c r="M153" s="10"/>
+      <c r="L153" s="10">
+        <v>1</v>
+      </c>
+      <c r="M153" s="10">
+        <v>1</v>
+      </c>
       <c r="N153" s="10"/>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
@@ -8773,8 +9379,12 @@
       <c r="K154" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L154" s="10"/>
-      <c r="M154" s="10"/>
+      <c r="L154" s="10">
+        <v>1</v>
+      </c>
+      <c r="M154" s="10">
+        <v>1</v>
+      </c>
       <c r="N154" s="10"/>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
@@ -8809,8 +9419,12 @@
       <c r="K155" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L155" s="10"/>
-      <c r="M155" s="10"/>
+      <c r="L155" s="10">
+        <v>1</v>
+      </c>
+      <c r="M155" s="10">
+        <v>1</v>
+      </c>
       <c r="N155" s="10"/>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
@@ -8845,8 +9459,12 @@
       <c r="K156" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L156" s="10"/>
-      <c r="M156" s="10"/>
+      <c r="L156" s="10">
+        <v>1</v>
+      </c>
+      <c r="M156" s="10">
+        <v>1</v>
+      </c>
       <c r="N156" s="10"/>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
@@ -8881,8 +9499,12 @@
       <c r="K157" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L157" s="10"/>
-      <c r="M157" s="10"/>
+      <c r="L157" s="10">
+        <v>1</v>
+      </c>
+      <c r="M157" s="10">
+        <v>1</v>
+      </c>
       <c r="N157" s="10"/>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
@@ -8917,8 +9539,12 @@
       <c r="K158" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L158" s="10"/>
-      <c r="M158" s="10"/>
+      <c r="L158" s="10">
+        <v>1</v>
+      </c>
+      <c r="M158" s="10">
+        <v>1</v>
+      </c>
       <c r="N158" s="10"/>
     </row>
   </sheetData>
@@ -8931,7 +9557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9020,8 +9648,12 @@
       <c r="K2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9056,8 +9688,12 @@
       <c r="K3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="L3" s="6">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9092,8 +9728,12 @@
       <c r="K4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -9128,8 +9768,12 @@
       <c r="K5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="L5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -9164,8 +9808,12 @@
       <c r="K6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -9200,8 +9848,12 @@
       <c r="K7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -9236,8 +9888,12 @@
       <c r="K8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -9272,8 +9928,12 @@
       <c r="K9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="6">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
       <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -9308,8 +9968,12 @@
       <c r="K10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
       <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -9344,8 +10008,12 @@
       <c r="K11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -9380,8 +10048,12 @@
       <c r="K12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -9416,8 +10088,12 @@
       <c r="K13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="L13" s="6">
+        <v>1</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -9452,8 +10128,12 @@
       <c r="K14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="L14" s="6">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -9488,8 +10168,12 @@
       <c r="K15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="L15" s="6">
+        <v>1</v>
+      </c>
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -9524,8 +10208,12 @@
       <c r="K16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="L16" s="6">
+        <v>1</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -9560,8 +10248,12 @@
       <c r="K17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="L17" s="6">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -9596,8 +10288,12 @@
       <c r="K18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="L18" s="6">
+        <v>1</v>
+      </c>
+      <c r="M18" s="6">
+        <v>1</v>
+      </c>
       <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -9632,8 +10328,12 @@
       <c r="K19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="L19" s="6">
+        <v>1</v>
+      </c>
+      <c r="M19" s="6">
+        <v>1</v>
+      </c>
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -9668,8 +10368,12 @@
       <c r="K20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="L20" s="6">
+        <v>1</v>
+      </c>
+      <c r="M20" s="6">
+        <v>1</v>
+      </c>
       <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -9704,8 +10408,12 @@
       <c r="K21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="L21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1</v>
+      </c>
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -9740,8 +10448,12 @@
       <c r="K22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="L22" s="6">
+        <v>1</v>
+      </c>
+      <c r="M22" s="6">
+        <v>1</v>
+      </c>
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -9776,8 +10488,12 @@
       <c r="K23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="L23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6">
+        <v>1</v>
+      </c>
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -9812,8 +10528,12 @@
       <c r="K24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
+        <v>1</v>
+      </c>
       <c r="N24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -9848,8 +10568,12 @@
       <c r="K25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6">
+        <v>1</v>
+      </c>
+      <c r="M25" s="6">
+        <v>1</v>
+      </c>
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -9884,8 +10608,12 @@
       <c r="K26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="L26" s="6">
+        <v>1</v>
+      </c>
+      <c r="M26" s="6">
+        <v>1</v>
+      </c>
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -9920,8 +10648,12 @@
       <c r="K27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="L27" s="6">
+        <v>1</v>
+      </c>
+      <c r="M27" s="6">
+        <v>1</v>
+      </c>
       <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -9956,8 +10688,12 @@
       <c r="K28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="L28" s="6">
+        <v>1</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -9992,8 +10728,12 @@
       <c r="K29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="L29" s="6">
+        <v>1</v>
+      </c>
+      <c r="M29" s="6">
+        <v>1</v>
+      </c>
       <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -10028,8 +10768,12 @@
       <c r="K30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="L30" s="6">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
+        <v>1</v>
+      </c>
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -10064,8 +10808,12 @@
       <c r="K31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="L31" s="6">
+        <v>1</v>
+      </c>
+      <c r="M31" s="6">
+        <v>1</v>
+      </c>
       <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -10100,8 +10848,12 @@
       <c r="K32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
+      <c r="L32" s="6">
+        <v>1</v>
+      </c>
+      <c r="M32" s="6">
+        <v>1</v>
+      </c>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -10136,8 +10888,12 @@
       <c r="K33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
+      <c r="L33" s="6">
+        <v>1</v>
+      </c>
+      <c r="M33" s="6">
+        <v>1</v>
+      </c>
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -10172,8 +10928,12 @@
       <c r="K34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
+      <c r="L34" s="6">
+        <v>1</v>
+      </c>
+      <c r="M34" s="6">
+        <v>1</v>
+      </c>
       <c r="N34" s="6"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -10208,8 +10968,12 @@
       <c r="K35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
+      <c r="L35" s="6">
+        <v>1</v>
+      </c>
+      <c r="M35" s="6">
+        <v>1</v>
+      </c>
       <c r="N35" s="6"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -10244,8 +11008,12 @@
       <c r="K36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
+      <c r="L36" s="6">
+        <v>1</v>
+      </c>
+      <c r="M36" s="6">
+        <v>1</v>
+      </c>
       <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -10280,8 +11048,12 @@
       <c r="K37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
+      <c r="L37" s="6">
+        <v>1</v>
+      </c>
+      <c r="M37" s="6">
+        <v>1</v>
+      </c>
       <c r="N37" s="6"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -10316,8 +11088,12 @@
       <c r="K38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
+      <c r="L38" s="6">
+        <v>1</v>
+      </c>
+      <c r="M38" s="6">
+        <v>1</v>
+      </c>
       <c r="N38" s="6"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -10352,8 +11128,12 @@
       <c r="K39" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
+      <c r="L39" s="6">
+        <v>1</v>
+      </c>
+      <c r="M39" s="6">
+        <v>1</v>
+      </c>
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -10388,8 +11168,12 @@
       <c r="K40" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
+      <c r="L40" s="6">
+        <v>1</v>
+      </c>
+      <c r="M40" s="6">
+        <v>1</v>
+      </c>
       <c r="N40" s="6"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -10424,8 +11208,12 @@
       <c r="K41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
+      <c r="L41" s="6">
+        <v>1</v>
+      </c>
+      <c r="M41" s="6">
+        <v>1</v>
+      </c>
       <c r="N41" s="6"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -10460,8 +11248,12 @@
       <c r="K42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
+      <c r="L42" s="6">
+        <v>1</v>
+      </c>
+      <c r="M42" s="6">
+        <v>1</v>
+      </c>
       <c r="N42" s="6"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -10496,8 +11288,12 @@
       <c r="K43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
+      <c r="L43" s="6">
+        <v>1</v>
+      </c>
+      <c r="M43" s="6">
+        <v>1</v>
+      </c>
       <c r="N43" s="6"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -10532,8 +11328,12 @@
       <c r="K44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
+      <c r="L44" s="6">
+        <v>1</v>
+      </c>
+      <c r="M44" s="6">
+        <v>1</v>
+      </c>
       <c r="N44" s="6"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -10568,8 +11368,12 @@
       <c r="K45" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
+      <c r="L45" s="6">
+        <v>1</v>
+      </c>
+      <c r="M45" s="6">
+        <v>1</v>
+      </c>
       <c r="N45" s="6"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -10604,8 +11408,12 @@
       <c r="K46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
+      <c r="L46" s="6">
+        <v>1</v>
+      </c>
+      <c r="M46" s="6">
+        <v>1</v>
+      </c>
       <c r="N46" s="6"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -10640,8 +11448,12 @@
       <c r="K47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
+      <c r="L47" s="6">
+        <v>1</v>
+      </c>
+      <c r="M47" s="6">
+        <v>1</v>
+      </c>
       <c r="N47" s="6"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -10676,8 +11488,12 @@
       <c r="K48" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
+      <c r="L48" s="6">
+        <v>1</v>
+      </c>
+      <c r="M48" s="6">
+        <v>1</v>
+      </c>
       <c r="N48" s="6"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -10712,8 +11528,12 @@
       <c r="K49" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
+      <c r="L49" s="6">
+        <v>1</v>
+      </c>
+      <c r="M49" s="6">
+        <v>1</v>
+      </c>
       <c r="N49" s="6"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -10748,8 +11568,12 @@
       <c r="K50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
+      <c r="L50" s="6">
+        <v>1</v>
+      </c>
+      <c r="M50" s="6">
+        <v>1</v>
+      </c>
       <c r="N50" s="6"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -10784,8 +11608,12 @@
       <c r="K51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
+      <c r="L51" s="6">
+        <v>1</v>
+      </c>
+      <c r="M51" s="6">
+        <v>1</v>
+      </c>
       <c r="N51" s="6"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -10820,8 +11648,12 @@
       <c r="K52" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
+      <c r="L52" s="6">
+        <v>1</v>
+      </c>
+      <c r="M52" s="6">
+        <v>1</v>
+      </c>
       <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -10856,8 +11688,12 @@
       <c r="K53" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
+      <c r="L53" s="6">
+        <v>1</v>
+      </c>
+      <c r="M53" s="6">
+        <v>1</v>
+      </c>
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -10892,8 +11728,12 @@
       <c r="K54" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
+      <c r="L54" s="6">
+        <v>1</v>
+      </c>
+      <c r="M54" s="6">
+        <v>1</v>
+      </c>
       <c r="N54" s="6"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -10928,8 +11768,12 @@
       <c r="K55" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
+      <c r="L55" s="6">
+        <v>1</v>
+      </c>
+      <c r="M55" s="6">
+        <v>1</v>
+      </c>
       <c r="N55" s="6"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -10964,8 +11808,12 @@
       <c r="K56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
+      <c r="L56" s="6">
+        <v>1</v>
+      </c>
+      <c r="M56" s="6">
+        <v>1</v>
+      </c>
       <c r="N56" s="6"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -11000,8 +11848,12 @@
       <c r="K57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
+      <c r="L57" s="6">
+        <v>1</v>
+      </c>
+      <c r="M57" s="6">
+        <v>1</v>
+      </c>
       <c r="N57" s="6"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -11036,8 +11888,12 @@
       <c r="K58" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
+      <c r="L58" s="6">
+        <v>1</v>
+      </c>
+      <c r="M58" s="6">
+        <v>1</v>
+      </c>
       <c r="N58" s="6"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -11072,8 +11928,12 @@
       <c r="K59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L59" s="6"/>
-      <c r="M59" s="6"/>
+      <c r="L59" s="6">
+        <v>1</v>
+      </c>
+      <c r="M59" s="6">
+        <v>1</v>
+      </c>
       <c r="N59" s="6"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -11108,8 +11968,12 @@
       <c r="K60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L60" s="6"/>
-      <c r="M60" s="6"/>
+      <c r="L60" s="6">
+        <v>1</v>
+      </c>
+      <c r="M60" s="6">
+        <v>1</v>
+      </c>
       <c r="N60" s="6"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -11144,8 +12008,12 @@
       <c r="K61" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
+      <c r="L61" s="6">
+        <v>1</v>
+      </c>
+      <c r="M61" s="6">
+        <v>1</v>
+      </c>
       <c r="N61" s="6"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -11180,8 +12048,12 @@
       <c r="K62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
+      <c r="L62" s="6">
+        <v>1</v>
+      </c>
+      <c r="M62" s="6">
+        <v>1</v>
+      </c>
       <c r="N62" s="6"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -11216,8 +12088,12 @@
       <c r="K63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L63" s="6"/>
-      <c r="M63" s="6"/>
+      <c r="L63" s="6">
+        <v>1</v>
+      </c>
+      <c r="M63" s="6">
+        <v>1</v>
+      </c>
       <c r="N63" s="6"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -11252,8 +12128,12 @@
       <c r="K64" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
+      <c r="L64" s="6">
+        <v>1</v>
+      </c>
+      <c r="M64" s="6">
+        <v>1</v>
+      </c>
       <c r="N64" s="6"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -11288,8 +12168,12 @@
       <c r="K65" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
+      <c r="L65" s="6">
+        <v>1</v>
+      </c>
+      <c r="M65" s="6">
+        <v>1</v>
+      </c>
       <c r="N65" s="6"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -11324,8 +12208,12 @@
       <c r="K66" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
+      <c r="L66" s="6">
+        <v>1</v>
+      </c>
+      <c r="M66" s="6">
+        <v>1</v>
+      </c>
       <c r="N66" s="6"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -11360,8 +12248,12 @@
       <c r="K67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L67" s="6"/>
-      <c r="M67" s="6"/>
+      <c r="L67" s="6">
+        <v>1</v>
+      </c>
+      <c r="M67" s="6">
+        <v>1</v>
+      </c>
       <c r="N67" s="6"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -11396,8 +12288,12 @@
       <c r="K68" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
+      <c r="L68" s="6">
+        <v>1</v>
+      </c>
+      <c r="M68" s="6">
+        <v>1</v>
+      </c>
       <c r="N68" s="6"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -11432,8 +12328,12 @@
       <c r="K69" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
+      <c r="L69" s="6">
+        <v>1</v>
+      </c>
+      <c r="M69" s="6">
+        <v>1</v>
+      </c>
       <c r="N69" s="6"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -11468,8 +12368,12 @@
       <c r="K70" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
+      <c r="L70" s="6">
+        <v>1</v>
+      </c>
+      <c r="M70" s="6">
+        <v>1</v>
+      </c>
       <c r="N70" s="6"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -11504,8 +12408,12 @@
       <c r="K71" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
+      <c r="L71" s="6">
+        <v>1</v>
+      </c>
+      <c r="M71" s="6">
+        <v>1</v>
+      </c>
       <c r="N71" s="6"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -11540,8 +12448,12 @@
       <c r="K72" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
+      <c r="L72" s="6">
+        <v>1</v>
+      </c>
+      <c r="M72" s="6">
+        <v>1</v>
+      </c>
       <c r="N72" s="6"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -11576,8 +12488,12 @@
       <c r="K73" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
+      <c r="L73" s="6">
+        <v>1</v>
+      </c>
+      <c r="M73" s="6">
+        <v>1</v>
+      </c>
       <c r="N73" s="6"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -11612,8 +12528,12 @@
       <c r="K74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
+      <c r="L74" s="6">
+        <v>1</v>
+      </c>
+      <c r="M74" s="6">
+        <v>1</v>
+      </c>
       <c r="N74" s="6"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -11648,8 +12568,12 @@
       <c r="K75" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
+      <c r="L75" s="6">
+        <v>1</v>
+      </c>
+      <c r="M75" s="6">
+        <v>1</v>
+      </c>
       <c r="N75" s="6"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -11684,8 +12608,12 @@
       <c r="K76" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
+      <c r="L76" s="6">
+        <v>1</v>
+      </c>
+      <c r="M76" s="6">
+        <v>1</v>
+      </c>
       <c r="N76" s="6"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -11720,8 +12648,12 @@
       <c r="K77" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
+      <c r="L77" s="6">
+        <v>1</v>
+      </c>
+      <c r="M77" s="6">
+        <v>1</v>
+      </c>
       <c r="N77" s="6"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -11756,8 +12688,12 @@
       <c r="K78" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
+      <c r="L78" s="6">
+        <v>1</v>
+      </c>
+      <c r="M78" s="6">
+        <v>1</v>
+      </c>
       <c r="N78" s="6"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -11792,8 +12728,12 @@
       <c r="K79" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
+      <c r="L79" s="6">
+        <v>1</v>
+      </c>
+      <c r="M79" s="6">
+        <v>1</v>
+      </c>
       <c r="N79" s="6"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -11828,8 +12768,12 @@
       <c r="K80" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
+      <c r="L80" s="6">
+        <v>1</v>
+      </c>
+      <c r="M80" s="6">
+        <v>1</v>
+      </c>
       <c r="N80" s="6"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -11864,8 +12808,12 @@
       <c r="K81" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
+      <c r="L81" s="6">
+        <v>1</v>
+      </c>
+      <c r="M81" s="6">
+        <v>1</v>
+      </c>
       <c r="N81" s="6"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -11900,8 +12848,12 @@
       <c r="K82" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L82" s="6"/>
-      <c r="M82" s="6"/>
+      <c r="L82" s="6">
+        <v>1</v>
+      </c>
+      <c r="M82" s="6">
+        <v>1</v>
+      </c>
       <c r="N82" s="6"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -11936,8 +12888,12 @@
       <c r="K83" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L83" s="6"/>
-      <c r="M83" s="6"/>
+      <c r="L83" s="6">
+        <v>1</v>
+      </c>
+      <c r="M83" s="6">
+        <v>1</v>
+      </c>
       <c r="N83" s="6"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -11972,8 +12928,12 @@
       <c r="K84" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
+      <c r="L84" s="6">
+        <v>1</v>
+      </c>
+      <c r="M84" s="6">
+        <v>1</v>
+      </c>
       <c r="N84" s="6"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -12008,8 +12968,12 @@
       <c r="K85" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L85" s="6"/>
-      <c r="M85" s="6"/>
+      <c r="L85" s="6">
+        <v>1</v>
+      </c>
+      <c r="M85" s="6">
+        <v>1</v>
+      </c>
       <c r="N85" s="6"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -12044,8 +13008,12 @@
       <c r="K86" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L86" s="6"/>
-      <c r="M86" s="6"/>
+      <c r="L86" s="6">
+        <v>1</v>
+      </c>
+      <c r="M86" s="6">
+        <v>1</v>
+      </c>
       <c r="N86" s="6"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -12080,8 +13048,12 @@
       <c r="K87" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L87" s="6"/>
-      <c r="M87" s="6"/>
+      <c r="L87" s="6">
+        <v>1</v>
+      </c>
+      <c r="M87" s="6">
+        <v>1</v>
+      </c>
       <c r="N87" s="6"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -12116,8 +13088,12 @@
       <c r="K88" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L88" s="6"/>
-      <c r="M88" s="6"/>
+      <c r="L88" s="6">
+        <v>1</v>
+      </c>
+      <c r="M88" s="6">
+        <v>1</v>
+      </c>
       <c r="N88" s="6"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -12152,8 +13128,12 @@
       <c r="K89" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L89" s="6"/>
-      <c r="M89" s="6"/>
+      <c r="L89" s="6">
+        <v>1</v>
+      </c>
+      <c r="M89" s="6">
+        <v>1</v>
+      </c>
       <c r="N89" s="6"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -12188,8 +13168,12 @@
       <c r="K90" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L90" s="6"/>
-      <c r="M90" s="6"/>
+      <c r="L90" s="6">
+        <v>1</v>
+      </c>
+      <c r="M90" s="6">
+        <v>1</v>
+      </c>
       <c r="N90" s="6"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -12224,8 +13208,12 @@
       <c r="K91" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L91" s="6"/>
-      <c r="M91" s="6"/>
+      <c r="L91" s="6">
+        <v>1</v>
+      </c>
+      <c r="M91" s="6">
+        <v>1</v>
+      </c>
       <c r="N91" s="6"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -12260,8 +13248,12 @@
       <c r="K92" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L92" s="6"/>
-      <c r="M92" s="6"/>
+      <c r="L92" s="6">
+        <v>1</v>
+      </c>
+      <c r="M92" s="6">
+        <v>1</v>
+      </c>
       <c r="N92" s="6"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -12296,8 +13288,12 @@
       <c r="K93" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L93" s="6"/>
-      <c r="M93" s="6"/>
+      <c r="L93" s="6">
+        <v>1</v>
+      </c>
+      <c r="M93" s="6">
+        <v>1</v>
+      </c>
       <c r="N93" s="6"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -12332,8 +13328,12 @@
       <c r="K94" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L94" s="6"/>
-      <c r="M94" s="6"/>
+      <c r="L94" s="6">
+        <v>1</v>
+      </c>
+      <c r="M94" s="6">
+        <v>1</v>
+      </c>
       <c r="N94" s="6"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -12368,8 +13368,12 @@
       <c r="K95" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L95" s="6"/>
-      <c r="M95" s="6"/>
+      <c r="L95" s="6">
+        <v>1</v>
+      </c>
+      <c r="M95" s="6">
+        <v>1</v>
+      </c>
       <c r="N95" s="6"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -12404,8 +13408,12 @@
       <c r="K96" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L96" s="6"/>
-      <c r="M96" s="6"/>
+      <c r="L96" s="6">
+        <v>1</v>
+      </c>
+      <c r="M96" s="6">
+        <v>1</v>
+      </c>
       <c r="N96" s="6"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -12440,8 +13448,12 @@
       <c r="K97" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L97" s="6"/>
-      <c r="M97" s="6"/>
+      <c r="L97" s="6">
+        <v>1</v>
+      </c>
+      <c r="M97" s="6">
+        <v>1</v>
+      </c>
       <c r="N97" s="6"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -12476,8 +13488,12 @@
       <c r="K98" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L98" s="6"/>
-      <c r="M98" s="6"/>
+      <c r="L98" s="6">
+        <v>1</v>
+      </c>
+      <c r="M98" s="6">
+        <v>1</v>
+      </c>
       <c r="N98" s="6"/>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -12512,8 +13528,12 @@
       <c r="K99" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L99" s="6"/>
-      <c r="M99" s="6"/>
+      <c r="L99" s="6">
+        <v>1</v>
+      </c>
+      <c r="M99" s="6">
+        <v>1</v>
+      </c>
       <c r="N99" s="6"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -12548,8 +13568,12 @@
       <c r="K100" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L100" s="6"/>
-      <c r="M100" s="6"/>
+      <c r="L100" s="6">
+        <v>1</v>
+      </c>
+      <c r="M100" s="6">
+        <v>1</v>
+      </c>
       <c r="N100" s="6"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -12584,8 +13608,12 @@
       <c r="K101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
+      <c r="L101" s="6">
+        <v>1</v>
+      </c>
+      <c r="M101" s="6">
+        <v>1</v>
+      </c>
       <c r="N101" s="6"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -12620,8 +13648,12 @@
       <c r="K102" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
+      <c r="L102" s="6">
+        <v>1</v>
+      </c>
+      <c r="M102" s="6">
+        <v>1</v>
+      </c>
       <c r="N102" s="6"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -12656,8 +13688,12 @@
       <c r="K103" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L103" s="6"/>
-      <c r="M103" s="6"/>
+      <c r="L103" s="6">
+        <v>1</v>
+      </c>
+      <c r="M103" s="6">
+        <v>1</v>
+      </c>
       <c r="N103" s="6"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -12692,8 +13728,12 @@
       <c r="K104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L104" s="6"/>
-      <c r="M104" s="6"/>
+      <c r="L104" s="6">
+        <v>1</v>
+      </c>
+      <c r="M104" s="6">
+        <v>1</v>
+      </c>
       <c r="N104" s="6"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -12728,8 +13768,12 @@
       <c r="K105" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L105" s="6"/>
-      <c r="M105" s="6"/>
+      <c r="L105" s="6">
+        <v>1</v>
+      </c>
+      <c r="M105" s="6">
+        <v>1</v>
+      </c>
       <c r="N105" s="6"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -12764,8 +13808,12 @@
       <c r="K106" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L106" s="6"/>
-      <c r="M106" s="6"/>
+      <c r="L106" s="6">
+        <v>1</v>
+      </c>
+      <c r="M106" s="6">
+        <v>1</v>
+      </c>
       <c r="N106" s="6"/>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -12800,8 +13848,12 @@
       <c r="K107" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L107" s="6"/>
-      <c r="M107" s="6"/>
+      <c r="L107" s="6">
+        <v>1</v>
+      </c>
+      <c r="M107" s="6">
+        <v>1</v>
+      </c>
       <c r="N107" s="6"/>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -12836,8 +13888,12 @@
       <c r="K108" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L108" s="6"/>
-      <c r="M108" s="6"/>
+      <c r="L108" s="6">
+        <v>1</v>
+      </c>
+      <c r="M108" s="6">
+        <v>1</v>
+      </c>
       <c r="N108" s="6"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -12872,8 +13928,12 @@
       <c r="K109" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L109" s="6"/>
-      <c r="M109" s="6"/>
+      <c r="L109" s="6">
+        <v>1</v>
+      </c>
+      <c r="M109" s="6">
+        <v>1</v>
+      </c>
       <c r="N109" s="6"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -12908,8 +13968,12 @@
       <c r="K110" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L110" s="6"/>
-      <c r="M110" s="6"/>
+      <c r="L110" s="6">
+        <v>1</v>
+      </c>
+      <c r="M110" s="6">
+        <v>1</v>
+      </c>
       <c r="N110" s="6"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -12944,8 +14008,12 @@
       <c r="K111" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L111" s="6"/>
-      <c r="M111" s="6"/>
+      <c r="L111" s="6">
+        <v>1</v>
+      </c>
+      <c r="M111" s="6">
+        <v>1</v>
+      </c>
       <c r="N111" s="6"/>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -12980,8 +14048,12 @@
       <c r="K112" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L112" s="6"/>
-      <c r="M112" s="6"/>
+      <c r="L112" s="6">
+        <v>1</v>
+      </c>
+      <c r="M112" s="6">
+        <v>1</v>
+      </c>
       <c r="N112" s="6"/>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -13016,8 +14088,12 @@
       <c r="K113" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L113" s="6"/>
-      <c r="M113" s="6"/>
+      <c r="L113" s="6">
+        <v>1</v>
+      </c>
+      <c r="M113" s="6">
+        <v>1</v>
+      </c>
       <c r="N113" s="6"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -13052,8 +14128,12 @@
       <c r="K114" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L114" s="6"/>
-      <c r="M114" s="6"/>
+      <c r="L114" s="6">
+        <v>1</v>
+      </c>
+      <c r="M114" s="6">
+        <v>1</v>
+      </c>
       <c r="N114" s="6"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -13088,8 +14168,12 @@
       <c r="K115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L115" s="6"/>
-      <c r="M115" s="6"/>
+      <c r="L115" s="6">
+        <v>1</v>
+      </c>
+      <c r="M115" s="6">
+        <v>1</v>
+      </c>
       <c r="N115" s="6"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -13124,8 +14208,12 @@
       <c r="K116" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
+      <c r="L116" s="6">
+        <v>1</v>
+      </c>
+      <c r="M116" s="6">
+        <v>1</v>
+      </c>
       <c r="N116" s="6"/>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -13160,8 +14248,12 @@
       <c r="K117" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L117" s="6"/>
-      <c r="M117" s="6"/>
+      <c r="L117" s="6">
+        <v>1</v>
+      </c>
+      <c r="M117" s="6">
+        <v>1</v>
+      </c>
       <c r="N117" s="6"/>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -13196,8 +14288,12 @@
       <c r="K118" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L118" s="6"/>
-      <c r="M118" s="6"/>
+      <c r="L118" s="6">
+        <v>1</v>
+      </c>
+      <c r="M118" s="6">
+        <v>1</v>
+      </c>
       <c r="N118" s="6"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -13232,8 +14328,12 @@
       <c r="K119" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L119" s="6"/>
-      <c r="M119" s="6"/>
+      <c r="L119" s="6">
+        <v>1</v>
+      </c>
+      <c r="M119" s="6">
+        <v>1</v>
+      </c>
       <c r="N119" s="6"/>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -13268,8 +14368,12 @@
       <c r="K120" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L120" s="6"/>
-      <c r="M120" s="6"/>
+      <c r="L120" s="6">
+        <v>1</v>
+      </c>
+      <c r="M120" s="6">
+        <v>1</v>
+      </c>
       <c r="N120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -13304,8 +14408,12 @@
       <c r="K121" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L121" s="6"/>
-      <c r="M121" s="6"/>
+      <c r="L121" s="6">
+        <v>1</v>
+      </c>
+      <c r="M121" s="6">
+        <v>1</v>
+      </c>
       <c r="N121" s="6"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -13340,8 +14448,12 @@
       <c r="K122" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L122" s="6"/>
-      <c r="M122" s="6"/>
+      <c r="L122" s="6">
+        <v>1</v>
+      </c>
+      <c r="M122" s="6">
+        <v>1</v>
+      </c>
       <c r="N122" s="6"/>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -13376,8 +14488,12 @@
       <c r="K123" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L123" s="6"/>
-      <c r="M123" s="6"/>
+      <c r="L123" s="6">
+        <v>1</v>
+      </c>
+      <c r="M123" s="6">
+        <v>1</v>
+      </c>
       <c r="N123" s="6"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
@@ -13412,8 +14528,12 @@
       <c r="K124" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L124" s="6"/>
-      <c r="M124" s="6"/>
+      <c r="L124" s="6">
+        <v>1</v>
+      </c>
+      <c r="M124" s="6">
+        <v>1</v>
+      </c>
       <c r="N124" s="6"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -13448,8 +14568,12 @@
       <c r="K125" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L125" s="6"/>
-      <c r="M125" s="6"/>
+      <c r="L125" s="6">
+        <v>1</v>
+      </c>
+      <c r="M125" s="6">
+        <v>1</v>
+      </c>
       <c r="N125" s="6"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -13484,8 +14608,12 @@
       <c r="K126" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L126" s="6"/>
-      <c r="M126" s="6"/>
+      <c r="L126" s="6">
+        <v>1</v>
+      </c>
+      <c r="M126" s="6">
+        <v>1</v>
+      </c>
       <c r="N126" s="6"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -13520,8 +14648,12 @@
       <c r="K127" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L127" s="6"/>
-      <c r="M127" s="6"/>
+      <c r="L127" s="6">
+        <v>1</v>
+      </c>
+      <c r="M127" s="6">
+        <v>1</v>
+      </c>
       <c r="N127" s="6"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -13556,8 +14688,12 @@
       <c r="K128" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L128" s="6"/>
-      <c r="M128" s="6"/>
+      <c r="L128" s="6">
+        <v>1</v>
+      </c>
+      <c r="M128" s="6">
+        <v>1</v>
+      </c>
       <c r="N128" s="6"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -13592,8 +14728,12 @@
       <c r="K129" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L129" s="6"/>
-      <c r="M129" s="6"/>
+      <c r="L129" s="6">
+        <v>1</v>
+      </c>
+      <c r="M129" s="6">
+        <v>1</v>
+      </c>
       <c r="N129" s="6"/>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -13628,8 +14768,12 @@
       <c r="K130" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L130" s="6"/>
-      <c r="M130" s="6"/>
+      <c r="L130" s="6">
+        <v>1</v>
+      </c>
+      <c r="M130" s="6">
+        <v>1</v>
+      </c>
       <c r="N130" s="6"/>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -13664,8 +14808,12 @@
       <c r="K131" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L131" s="6"/>
-      <c r="M131" s="6"/>
+      <c r="L131" s="6">
+        <v>1</v>
+      </c>
+      <c r="M131" s="6">
+        <v>1</v>
+      </c>
       <c r="N131" s="6"/>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -13700,8 +14848,12 @@
       <c r="K132" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L132" s="6"/>
-      <c r="M132" s="6"/>
+      <c r="L132" s="6">
+        <v>1</v>
+      </c>
+      <c r="M132" s="6">
+        <v>1</v>
+      </c>
       <c r="N132" s="6"/>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
@@ -13736,8 +14888,12 @@
       <c r="K133" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L133" s="6"/>
-      <c r="M133" s="6"/>
+      <c r="L133" s="6">
+        <v>1</v>
+      </c>
+      <c r="M133" s="6">
+        <v>1</v>
+      </c>
       <c r="N133" s="6"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -13772,8 +14928,12 @@
       <c r="K134" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L134" s="6"/>
-      <c r="M134" s="6"/>
+      <c r="L134" s="6">
+        <v>1</v>
+      </c>
+      <c r="M134" s="6">
+        <v>1</v>
+      </c>
       <c r="N134" s="6"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -13808,8 +14968,12 @@
       <c r="K135" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L135" s="6"/>
-      <c r="M135" s="6"/>
+      <c r="L135" s="6">
+        <v>1</v>
+      </c>
+      <c r="M135" s="6">
+        <v>1</v>
+      </c>
       <c r="N135" s="6"/>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -13844,8 +15008,12 @@
       <c r="K136" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L136" s="6"/>
-      <c r="M136" s="6"/>
+      <c r="L136" s="6">
+        <v>1</v>
+      </c>
+      <c r="M136" s="6">
+        <v>1</v>
+      </c>
       <c r="N136" s="6"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -13880,8 +15048,12 @@
       <c r="K137" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L137" s="6"/>
-      <c r="M137" s="6"/>
+      <c r="L137" s="6">
+        <v>1</v>
+      </c>
+      <c r="M137" s="6">
+        <v>1</v>
+      </c>
       <c r="N137" s="6"/>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -13916,8 +15088,12 @@
       <c r="K138" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L138" s="6"/>
-      <c r="M138" s="6"/>
+      <c r="L138" s="6">
+        <v>1</v>
+      </c>
+      <c r="M138" s="6">
+        <v>1</v>
+      </c>
       <c r="N138" s="6"/>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -13952,8 +15128,12 @@
       <c r="K139" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L139" s="6"/>
-      <c r="M139" s="6"/>
+      <c r="L139" s="6">
+        <v>1</v>
+      </c>
+      <c r="M139" s="6">
+        <v>1</v>
+      </c>
       <c r="N139" s="6"/>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -13988,8 +15168,12 @@
       <c r="K140" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L140" s="6"/>
-      <c r="M140" s="6"/>
+      <c r="L140" s="6">
+        <v>1</v>
+      </c>
+      <c r="M140" s="6">
+        <v>1</v>
+      </c>
       <c r="N140" s="6"/>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -14024,8 +15208,12 @@
       <c r="K141" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L141" s="6"/>
-      <c r="M141" s="6"/>
+      <c r="L141" s="6">
+        <v>1</v>
+      </c>
+      <c r="M141" s="6">
+        <v>1</v>
+      </c>
       <c r="N141" s="6"/>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
@@ -14060,8 +15248,12 @@
       <c r="K142" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L142" s="6"/>
-      <c r="M142" s="6"/>
+      <c r="L142" s="6">
+        <v>1</v>
+      </c>
+      <c r="M142" s="6">
+        <v>1</v>
+      </c>
       <c r="N142" s="6"/>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -14096,8 +15288,12 @@
       <c r="K143" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L143" s="6"/>
-      <c r="M143" s="6"/>
+      <c r="L143" s="6">
+        <v>1</v>
+      </c>
+      <c r="M143" s="6">
+        <v>1</v>
+      </c>
       <c r="N143" s="6"/>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -14132,8 +15328,12 @@
       <c r="K144" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L144" s="6"/>
-      <c r="M144" s="6"/>
+      <c r="L144" s="6">
+        <v>1</v>
+      </c>
+      <c r="M144" s="6">
+        <v>1</v>
+      </c>
       <c r="N144" s="6"/>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -14168,8 +15368,12 @@
       <c r="K145" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L145" s="6"/>
-      <c r="M145" s="6"/>
+      <c r="L145" s="6">
+        <v>1</v>
+      </c>
+      <c r="M145" s="6">
+        <v>1</v>
+      </c>
       <c r="N145" s="6"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -14204,8 +15408,12 @@
       <c r="K146" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L146" s="6"/>
-      <c r="M146" s="6"/>
+      <c r="L146" s="6">
+        <v>1</v>
+      </c>
+      <c r="M146" s="6">
+        <v>1</v>
+      </c>
       <c r="N146" s="6"/>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -14240,8 +15448,12 @@
       <c r="K147" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L147" s="6"/>
-      <c r="M147" s="6"/>
+      <c r="L147" s="6">
+        <v>1</v>
+      </c>
+      <c r="M147" s="6">
+        <v>1</v>
+      </c>
       <c r="N147" s="6"/>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -14276,8 +15488,12 @@
       <c r="K148" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L148" s="6"/>
-      <c r="M148" s="6"/>
+      <c r="L148" s="6">
+        <v>1</v>
+      </c>
+      <c r="M148" s="6">
+        <v>1</v>
+      </c>
       <c r="N148" s="6"/>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -14312,8 +15528,12 @@
       <c r="K149" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L149" s="6"/>
-      <c r="M149" s="6"/>
+      <c r="L149" s="6">
+        <v>1</v>
+      </c>
+      <c r="M149" s="6">
+        <v>1</v>
+      </c>
       <c r="N149" s="6"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -14348,8 +15568,12 @@
       <c r="K150" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L150" s="6"/>
-      <c r="M150" s="6"/>
+      <c r="L150" s="6">
+        <v>1</v>
+      </c>
+      <c r="M150" s="6">
+        <v>1</v>
+      </c>
       <c r="N150" s="6"/>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -14384,8 +15608,12 @@
       <c r="K151" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L151" s="6"/>
-      <c r="M151" s="6"/>
+      <c r="L151" s="6">
+        <v>1</v>
+      </c>
+      <c r="M151" s="6">
+        <v>1</v>
+      </c>
       <c r="N151" s="6"/>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
@@ -14420,8 +15648,12 @@
       <c r="K152" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L152" s="6"/>
-      <c r="M152" s="6"/>
+      <c r="L152" s="6">
+        <v>1</v>
+      </c>
+      <c r="M152" s="6">
+        <v>1</v>
+      </c>
       <c r="N152" s="6"/>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
@@ -14456,8 +15688,12 @@
       <c r="K153" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L153" s="6"/>
-      <c r="M153" s="6"/>
+      <c r="L153" s="6">
+        <v>1</v>
+      </c>
+      <c r="M153" s="6">
+        <v>1</v>
+      </c>
       <c r="N153" s="6"/>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
@@ -14492,8 +15728,12 @@
       <c r="K154" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L154" s="6"/>
-      <c r="M154" s="6"/>
+      <c r="L154" s="6">
+        <v>1</v>
+      </c>
+      <c r="M154" s="6">
+        <v>1</v>
+      </c>
       <c r="N154" s="6"/>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
@@ -14528,8 +15768,12 @@
       <c r="K155" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L155" s="6"/>
-      <c r="M155" s="6"/>
+      <c r="L155" s="6">
+        <v>1</v>
+      </c>
+      <c r="M155" s="6">
+        <v>1</v>
+      </c>
       <c r="N155" s="6"/>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
@@ -14564,8 +15808,12 @@
       <c r="K156" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L156" s="6"/>
-      <c r="M156" s="6"/>
+      <c r="L156" s="6">
+        <v>1</v>
+      </c>
+      <c r="M156" s="6">
+        <v>1</v>
+      </c>
       <c r="N156" s="6"/>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
@@ -14600,8 +15848,12 @@
       <c r="K157" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L157" s="6"/>
-      <c r="M157" s="6"/>
+      <c r="L157" s="6">
+        <v>1</v>
+      </c>
+      <c r="M157" s="6">
+        <v>1</v>
+      </c>
       <c r="N157" s="6"/>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
@@ -14636,8 +15888,12 @@
       <c r="K158" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L158" s="6"/>
-      <c r="M158" s="6"/>
+      <c r="L158" s="6">
+        <v>1</v>
+      </c>
+      <c r="M158" s="6">
+        <v>1</v>
+      </c>
       <c r="N158" s="6"/>
     </row>
   </sheetData>

</xml_diff>